<commit_message>
modificacion a documentos SENA
</commit_message>
<xml_diff>
--- a/SenaDocs/doc/trim5/Plan de implementacion/Plan de capacitacion/Ascpectos-verificar.xlsx
+++ b/SenaDocs/doc/trim5/Plan de implementacion/Plan de capacitacion/Ascpectos-verificar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FABIAN ESCOBAR VARGA\OneDrive\Fabian Escobar\Escritorio\Oscar personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE 314\Desktop\TPS_FDS-2671339-HS1\SenaDocs\doc\trim5\Plan de implementacion\Plan de capacitacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFAC5F4C-7008-4ECB-A7EA-A38AB2725631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70FE671-DEEA-4CC9-B031-ED45A54433E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" firstSheet="4" activeTab="4" xr2:uid="{DFBD055B-9E24-415E-AA77-0A6F31C85827}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{DFBD055B-9E24-415E-AA77-0A6F31C85827}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="Capacitación" sheetId="4" r:id="rId3"/>
     <sheet name="Documentación" sheetId="5" r:id="rId4"/>
     <sheet name="Soporte-tecnico" sheetId="6" r:id="rId5"/>
+    <sheet name="Hardware (2)" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Hardware (2)'!$B$1:$E$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="23">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -352,24 +356,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -405,6 +391,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EAB6B7-0F5F-48DB-9A8F-C1666FF40182}">
   <dimension ref="B1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -757,64 +761,64 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -828,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88A9CF0-B35D-4A9C-8B74-05F37614A97B}">
   <dimension ref="B1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,72 +847,72 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -923,7 +927,7 @@
   <dimension ref="B1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,64 +941,64 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1009,7 +1013,7 @@
   <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,56 +1027,56 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1086,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F812DEF-B51F-4536-91CD-1145EF7AFD4F}">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,56 +1105,56 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1158,4 +1162,334 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE11B464-0C60-4AA5-BE8F-284AC9D8AE24}">
+  <dimension ref="B1:E48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="84.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="44.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="B12:E13"/>
+    <mergeCell ref="B23:E24"/>
+    <mergeCell ref="B33:E34"/>
+    <mergeCell ref="B42:E43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="59" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="1" max="47" man="1"/>
+  </colBreaks>
+</worksheet>
 </file>
</xml_diff>